<commit_message>
Final plots for CCK8 assays
</commit_message>
<xml_diff>
--- a/CCK8_Assay_Plots/20230915_CellCulture_DIP70equivtransfection copy.xlsx
+++ b/CCK8_Assay_Plots/20230915_CellCulture_DIP70equivtransfection copy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mines0-my.sharepoint.com/personal/aryellewright_mines_edu/Documents/Research/Kumar Research Lab/Aryelle's Lab Notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mines0-my.sharepoint.com/personal/aryellewright_mines_edu/Documents/Research/Kumar Research Lab/Aryelle's Lab Notebook/CCK8 Plate Reader Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="11_2477821883FF8919E444A949EB56D535D014B8AF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CA9AA64-BFDD-7B41-AC6B-10AFF2A3CFCF}"/>
+  <xr:revisionPtr revIDLastSave="361" documentId="11_2477821883FF8919E444A949EB56D535D014B8AF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5B42A79-DCE1-6B47-9F35-FBE4D90498B0}"/>
   <bookViews>
-    <workbookView xWindow="-26000" yWindow="11200" windowWidth="25320" windowHeight="15980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="28800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="74">
   <si>
     <t>Software Version</t>
   </si>
@@ -170,9 +170,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>Absorbance at 720</t>
-  </si>
-  <si>
     <t>Absorbance at 460</t>
   </si>
   <si>
@@ -191,12 +188,6 @@
     <t>DIP70 N/P 1</t>
   </si>
   <si>
-    <t>DIP70 N/P 2.5</t>
-  </si>
-  <si>
-    <t>DIP70 N/P 5</t>
-  </si>
-  <si>
     <t>DIP70 N/P 10</t>
   </si>
   <si>
@@ -239,9 +230,6 @@
     <t>Well 3 Correction</t>
   </si>
   <si>
-    <t>Standard Deviation %</t>
-  </si>
-  <si>
     <t>StdDev</t>
   </si>
   <si>
@@ -254,23 +242,32 @@
     <t>Variables</t>
   </si>
   <si>
-    <t>N/P 1</t>
-  </si>
-  <si>
-    <t>N/P 2.5</t>
-  </si>
-  <si>
-    <t>N/P 5</t>
-  </si>
-  <si>
     <t>N/P 10</t>
+  </si>
+  <si>
+    <t>jetPEI</t>
+  </si>
+  <si>
+    <t>LPF2000</t>
+  </si>
+  <si>
+    <t>pDNA + water</t>
+  </si>
+  <si>
+    <t>Transfection</t>
+  </si>
+  <si>
+    <t>Usually 50-60% viability</t>
+  </si>
+  <si>
+    <t>Usually &gt;70% viability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -307,7 +304,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,8 +395,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -475,30 +478,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -511,11 +490,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -603,34 +593,58 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,18 +931,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O67"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:H51"/>
+    <sheetView topLeftCell="A26" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -936,17 +950,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -954,7 +968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -962,7 +976,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -970,7 +984,7 @@
         <v>0.66047453703703707</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -978,7 +992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -986,7 +1000,7 @@
         <v>14092513</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -994,13 +1008,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" ht="14">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1008,12 +1022,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1021,22 +1035,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="B17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="B18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="B19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1044,48 +1058,48 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="B21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="B22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="B23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="B24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="B25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="B26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="B27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" ht="14">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1093,7 +1107,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1101,7 +1115,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1109,7 +1123,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1117,7 +1131,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15">
       <c r="B35" s="5"/>
       <c r="C35" s="6">
         <v>1</v>
@@ -1154,8 +1168,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B36" s="31" t="s">
+    <row r="36" spans="1:15">
+      <c r="B36" s="38" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="7">
@@ -1198,8 +1212,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B37" s="32"/>
+    <row r="37" spans="1:15">
+      <c r="B37" s="39"/>
       <c r="C37" s="13">
         <v>0.41899999999999998</v>
       </c>
@@ -1240,8 +1254,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B38" s="32"/>
+    <row r="38" spans="1:15">
+      <c r="B38" s="39"/>
       <c r="C38" s="17">
         <v>4.1000000000000002E-2</v>
       </c>
@@ -1282,8 +1296,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B39" s="33"/>
+    <row r="39" spans="1:15" ht="36">
+      <c r="B39" s="40"/>
       <c r="C39" s="19">
         <v>104224</v>
       </c>
@@ -1324,8 +1338,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B40" s="31" t="s">
+    <row r="40" spans="1:15">
+      <c r="B40" s="38" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="7">
@@ -1368,8 +1382,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B41" s="32"/>
+    <row r="41" spans="1:15">
+      <c r="B41" s="39"/>
       <c r="C41" s="13">
         <v>0.373</v>
       </c>
@@ -1410,8 +1424,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B42" s="32"/>
+    <row r="42" spans="1:15">
+      <c r="B42" s="39"/>
       <c r="C42" s="17">
         <v>0.06</v>
       </c>
@@ -1452,8 +1466,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B43" s="33"/>
+    <row r="43" spans="1:15" ht="36">
+      <c r="B43" s="40"/>
       <c r="C43" s="24">
         <v>154316</v>
       </c>
@@ -1494,8 +1508,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B44" s="31" t="s">
+    <row r="44" spans="1:15">
+      <c r="B44" s="38" t="s">
         <v>37</v>
       </c>
       <c r="C44" s="7">
@@ -1538,8 +1552,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B45" s="32"/>
+    <row r="45" spans="1:15">
+      <c r="B45" s="39"/>
       <c r="C45" s="13">
         <v>0.44400000000000001</v>
       </c>
@@ -1580,8 +1594,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B46" s="32"/>
+    <row r="46" spans="1:15">
+      <c r="B46" s="39"/>
       <c r="C46" s="17">
         <v>0.04</v>
       </c>
@@ -1622,8 +1636,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B47" s="33"/>
+    <row r="47" spans="1:15" ht="36">
+      <c r="B47" s="40"/>
       <c r="C47" s="20">
         <v>95164</v>
       </c>
@@ -1664,8 +1678,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B48" s="31" t="s">
+    <row r="48" spans="1:15">
+      <c r="B48" s="38" t="s">
         <v>38</v>
       </c>
       <c r="C48" s="11">
@@ -1708,8 +1722,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B49" s="32"/>
+    <row r="49" spans="1:15">
+      <c r="B49" s="39"/>
       <c r="C49" s="17">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -1750,8 +1764,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B50" s="32"/>
+    <row r="50" spans="1:15">
+      <c r="A50">
+        <f>F48-F50</f>
+        <v>0.53</v>
+      </c>
+      <c r="B50" s="39"/>
       <c r="C50" s="17">
         <v>4.5999999999999999E-2</v>
       </c>
@@ -1792,8 +1810,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B51" s="33"/>
+    <row r="51" spans="1:15" ht="36">
+      <c r="B51" s="40"/>
       <c r="C51" s="21">
         <v>58726</v>
       </c>
@@ -1834,8 +1852,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B52" s="31" t="s">
+    <row r="52" spans="1:15">
+      <c r="B52" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C52" s="11">
@@ -1878,8 +1896,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B53" s="32"/>
+    <row r="53" spans="1:15">
+      <c r="B53" s="39"/>
       <c r="C53" s="17">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -1920,8 +1938,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B54" s="32"/>
+    <row r="54" spans="1:15">
+      <c r="B54" s="39"/>
       <c r="C54" s="17">
         <v>4.5999999999999999E-2</v>
       </c>
@@ -1962,8 +1980,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B55" s="33"/>
+    <row r="55" spans="1:15" ht="36">
+      <c r="B55" s="40"/>
       <c r="C55" s="21">
         <v>59177</v>
       </c>
@@ -2004,8 +2022,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B56" s="31" t="s">
+    <row r="56" spans="1:15">
+      <c r="B56" s="38" t="s">
         <v>40</v>
       </c>
       <c r="C56" s="11">
@@ -2048,8 +2066,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B57" s="32"/>
+    <row r="57" spans="1:15">
+      <c r="B57" s="39"/>
       <c r="C57" s="17">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -2090,8 +2108,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B58" s="32"/>
+    <row r="58" spans="1:15">
+      <c r="B58" s="39"/>
       <c r="C58" s="17">
         <v>4.3999999999999997E-2</v>
       </c>
@@ -2132,8 +2150,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B59" s="33"/>
+    <row r="59" spans="1:15" ht="36">
+      <c r="B59" s="40"/>
       <c r="C59" s="21">
         <v>61147</v>
       </c>
@@ -2174,8 +2192,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B60" s="31" t="s">
+    <row r="60" spans="1:15">
+      <c r="B60" s="38" t="s">
         <v>41</v>
       </c>
       <c r="C60" s="11">
@@ -2218,8 +2236,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B61" s="32"/>
+    <row r="61" spans="1:15">
+      <c r="B61" s="39"/>
       <c r="C61" s="17">
         <v>5.0999999999999997E-2</v>
       </c>
@@ -2260,8 +2278,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B62" s="32"/>
+    <row r="62" spans="1:15">
+      <c r="B62" s="39"/>
       <c r="C62" s="17">
         <v>4.3999999999999997E-2</v>
       </c>
@@ -2302,8 +2320,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B63" s="33"/>
+    <row r="63" spans="1:15" ht="36">
+      <c r="B63" s="40"/>
       <c r="C63" s="21">
         <v>60626</v>
       </c>
@@ -2344,8 +2362,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B64" s="31" t="s">
+    <row r="64" spans="1:15">
+      <c r="B64" s="38" t="s">
         <v>42</v>
       </c>
       <c r="C64" s="11">
@@ -2388,8 +2406,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B65" s="32"/>
+    <row r="65" spans="2:15">
+      <c r="B65" s="39"/>
       <c r="C65" s="17">
         <v>5.5E-2</v>
       </c>
@@ -2430,8 +2448,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.15">
-      <c r="B66" s="32"/>
+    <row r="66" spans="2:15">
+      <c r="B66" s="39"/>
       <c r="C66" s="17">
         <v>4.7E-2</v>
       </c>
@@ -2472,8 +2490,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="67" spans="2:15" ht="36" x14ac:dyDescent="0.15">
-      <c r="B67" s="33"/>
+    <row r="67" spans="2:15" ht="36">
+      <c r="B67" s="40"/>
       <c r="C67" s="21">
         <v>60947</v>
       </c>
@@ -2534,1017 +2552,821 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1DA1369-28CA-9043-A130-DDEE60AA999D}">
-  <dimension ref="B5:S54"/>
+  <dimension ref="B4:S51"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27:S34"/>
+    <sheetView topLeftCell="G1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" customWidth="1"/>
     <col min="13" max="13" width="12.83203125" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B5" s="34" t="s">
+    <row r="4" spans="2:17">
+      <c r="B4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="17">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="C6">
+        <f>AVERAGE(B4:B6)</f>
+        <v>4.1333333333333333E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="31"/>
+    </row>
+    <row r="8" spans="2:17" ht="42">
+      <c r="B8" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C5">
-        <v>4.7E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B7" s="34"/>
-    </row>
-    <row r="8" spans="2:17" ht="42" x14ac:dyDescent="0.15">
-      <c r="B8" s="34" t="s">
+      <c r="C8" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="O8" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="P8" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" s="33"/>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="O8" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="P8" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q8" s="43"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B9" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="C9" s="47">
         <v>0.43099999999999999</v>
       </c>
-      <c r="D9" s="8">
-        <v>0.81</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="48">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="E9" s="47">
         <v>0.42599999999999999</v>
       </c>
-      <c r="H9" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="7">
-        <f>C9-C$5</f>
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="J9" s="8">
-        <f>D9-C$5</f>
-        <v>0.76300000000000001</v>
-      </c>
-      <c r="K9" s="7">
-        <f>E9-C$5</f>
-        <v>0.379</v>
+      <c r="H9" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="47">
+        <f>C9-C$6</f>
+        <v>0.38966666666666666</v>
+      </c>
+      <c r="J9" s="48">
+        <f>D9-C$6</f>
+        <v>0.50766666666666671</v>
+      </c>
+      <c r="K9" s="47">
+        <f>E9-C$6</f>
+        <v>0.38466666666666666</v>
       </c>
       <c r="L9">
         <f>AVERAGE(I$9:K$9)</f>
-        <v>0.50866666666666671</v>
-      </c>
-      <c r="O9" s="41">
+        <v>0.42733333333333334</v>
+      </c>
+      <c r="O9" s="36">
         <f>L9/L$10</f>
-        <v>0.48598726114649687</v>
-      </c>
-      <c r="P9" s="41">
+        <v>0.85982562038900057</v>
+      </c>
+      <c r="P9" s="36">
         <f>100*O$9</f>
-        <v>48.598726114649686</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B10" s="34" t="s">
+        <v>85.982562038900056</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="49">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D10" s="53">
+        <v>0.56300000000000017</v>
+      </c>
+      <c r="E10" s="47">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="47">
+        <f>C10-C$6</f>
+        <v>0.51866666666666672</v>
+      </c>
+      <c r="J10" s="48">
+        <f>D10-C$6</f>
+        <v>0.52166666666666683</v>
+      </c>
+      <c r="K10" s="47">
+        <f>E10-C$6</f>
+        <v>0.45066666666666666</v>
+      </c>
+      <c r="L10" s="52">
+        <f>(I10+J10+K10)/3</f>
+        <v>0.49700000000000005</v>
+      </c>
+      <c r="M10" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="O10" s="36">
+        <f t="shared" ref="O10:O16" si="0">L10/L$10</f>
+        <v>1</v>
+      </c>
+      <c r="P10" s="36">
+        <f t="shared" ref="P10:P16" si="1">100*O10</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="9">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2.2290000000000001</v>
-      </c>
-      <c r="E10" s="7">
-        <v>0.49199999999999999</v>
-      </c>
-      <c r="H10" s="34" t="s">
+      <c r="C11" s="47">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="D11" s="50">
+        <v>0.308</v>
+      </c>
+      <c r="E11" s="50">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="H11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="7">
-        <f t="shared" ref="I10:I16" si="0">C10-C$5</f>
-        <v>0.51300000000000001</v>
-      </c>
-      <c r="J10" s="8">
-        <f t="shared" ref="J10:J16" si="1">D10-C$5</f>
-        <v>2.1819999999999999</v>
-      </c>
-      <c r="K10" s="38">
-        <f t="shared" ref="K10:K16" si="2">E10-C$5</f>
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="L10" s="44">
-        <f>(I10+J10+K10)/3</f>
-        <v>1.0466666666666666</v>
-      </c>
-      <c r="M10" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" s="41">
-        <f t="shared" ref="O10:O16" si="3">L10/L$10</f>
-        <v>1</v>
-      </c>
-      <c r="P10" s="41">
-        <f>100*O10</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B11" s="34" t="s">
+      <c r="I11" s="47">
+        <f>C11-C$6</f>
+        <v>0.34166666666666667</v>
+      </c>
+      <c r="J11" s="48">
+        <f>D11-C$6</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="K11" s="47">
+        <f>E11-C$6</f>
+        <v>0.25066666666666665</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:L16" si="2">AVERAGE(I11:K11)</f>
+        <v>0.28633333333333333</v>
+      </c>
+      <c r="O11" s="36">
+        <f t="shared" si="0"/>
+        <v>0.57612340710932253</v>
+      </c>
+      <c r="P11" s="36">
+        <f t="shared" si="1"/>
+        <v>57.612340710932251</v>
+      </c>
+      <c r="Q11" s="31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="B12" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="7">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="D11" s="23">
-        <v>0.308</v>
-      </c>
-      <c r="E11" s="23">
-        <v>0.29199999999999998</v>
-      </c>
-      <c r="H11" s="34" t="s">
+      <c r="C12" s="47">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="D12" s="47">
+        <v>0.51</v>
+      </c>
+      <c r="E12" s="47">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="H12" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I12" s="47">
+        <f>C12-C$6</f>
+        <v>0.37666666666666665</v>
+      </c>
+      <c r="J12" s="48">
+        <f>D12-C$6</f>
+        <v>0.46866666666666668</v>
+      </c>
+      <c r="K12" s="47">
+        <f>E12-C$6</f>
+        <v>0.42366666666666669</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="O12" s="36">
         <f t="shared" si="0"/>
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="J11" s="8">
+        <v>0.85110663983903412</v>
+      </c>
+      <c r="P12" s="36">
         <f t="shared" si="1"/>
-        <v>0.26100000000000001</v>
-      </c>
-      <c r="K11" s="7">
+        <v>85.110663983903407</v>
+      </c>
+      <c r="Q12" s="31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="B13" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="47">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="D13" s="47">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="E13" s="49">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="47">
+        <f>C13-C$6</f>
+        <v>0.41466666666666668</v>
+      </c>
+      <c r="J13" s="48">
+        <f>D13-C$6</f>
+        <v>0.44966666666666666</v>
+      </c>
+      <c r="K13" s="47">
+        <f>E13-C$6</f>
+        <v>0.54566666666666663</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="2"/>
-        <v>0.245</v>
-      </c>
-      <c r="L11">
-        <f>AVERAGE(I11:K11)</f>
-        <v>0.28066666666666668</v>
-      </c>
-      <c r="O11" s="41">
-        <f t="shared" si="3"/>
-        <v>0.26815286624203821</v>
-      </c>
-      <c r="P11" s="41">
-        <f>100*O11</f>
-        <v>26.815286624203821</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B12" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="7">
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0.51</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="H12" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="7">
+        <v>0.47000000000000003</v>
+      </c>
+      <c r="O13" s="36">
         <f t="shared" si="0"/>
-        <v>0.371</v>
-      </c>
-      <c r="J12" s="8">
+        <v>0.94567404426559354</v>
+      </c>
+      <c r="P13" s="36">
         <f t="shared" si="1"/>
-        <v>0.46300000000000002</v>
-      </c>
-      <c r="K12" s="7">
-        <f t="shared" si="2"/>
-        <v>0.41800000000000004</v>
-      </c>
-      <c r="L12">
-        <f>AVERAGE(I12:K12)</f>
-        <v>0.41733333333333339</v>
-      </c>
-      <c r="O12" s="41">
-        <f t="shared" si="3"/>
-        <v>0.39872611464968161</v>
-      </c>
-      <c r="P12" s="41">
-        <f>100*O12</f>
-        <v>39.872611464968159</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B13" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="7">
-        <v>0.45600000000000002</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0.58699999999999997</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.40900000000000003</v>
-      </c>
-      <c r="J13" s="8">
-        <f t="shared" si="1"/>
-        <v>0.44400000000000001</v>
-      </c>
-      <c r="K13" s="7">
-        <f t="shared" si="2"/>
-        <v>0.53999999999999992</v>
-      </c>
-      <c r="L13">
-        <f>AVERAGE(I13:K13)</f>
-        <v>0.46433333333333326</v>
-      </c>
-      <c r="O13" s="41">
-        <f t="shared" si="3"/>
-        <v>0.4436305732484076</v>
-      </c>
-      <c r="P13" s="41">
-        <f>100*O13</f>
-        <v>44.36305732484076</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B14" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="11">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="D14" s="11">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="E14" s="11">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="7">
-        <f t="shared" si="0"/>
-        <v>-3.0000000000000027E-3</v>
-      </c>
-      <c r="J14" s="8">
-        <f t="shared" si="1"/>
-        <v>-4.9999999999999975E-3</v>
-      </c>
-      <c r="K14" s="7">
-        <f t="shared" si="2"/>
-        <v>-3.0000000000000027E-3</v>
-      </c>
-      <c r="L14">
-        <f>AVERAGE(I14:K14)</f>
-        <v>-3.6666666666666675E-3</v>
-      </c>
-      <c r="O14" s="41">
-        <f t="shared" si="3"/>
-        <v>-3.5031847133757971E-3</v>
-      </c>
-      <c r="P14" s="41">
-        <f>100*O14</f>
-        <v>-0.35031847133757971</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B15" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="11">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="E15" s="11">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="H15" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="7">
-        <f t="shared" si="0"/>
-        <v>4.9999999999999975E-3</v>
-      </c>
-      <c r="J15" s="8">
-        <f t="shared" si="1"/>
-        <v>4.9999999999999975E-3</v>
-      </c>
-      <c r="K15" s="7">
-        <f t="shared" si="2"/>
-        <v>5.9999999999999984E-3</v>
-      </c>
-      <c r="L15">
-        <f>AVERAGE(I15:K15)</f>
-        <v>5.3333333333333314E-3</v>
-      </c>
-      <c r="O15" s="41">
-        <f t="shared" si="3"/>
-        <v>5.0955414012738834E-3</v>
-      </c>
-      <c r="P15" s="41">
-        <f>100*O15</f>
-        <v>0.50955414012738831</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.15">
-      <c r="B16" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="27">
-        <v>1.4470000000000001</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0.46100000000000002</v>
-      </c>
-      <c r="E16" s="7">
-        <v>0.44400000000000001</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4000000000000001</v>
-      </c>
-      <c r="J16" s="8">
-        <f t="shared" si="1"/>
-        <v>0.41400000000000003</v>
-      </c>
-      <c r="K16" s="7">
-        <f t="shared" si="2"/>
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="L16">
-        <f>AVERAGE(I16:K16)</f>
-        <v>0.7370000000000001</v>
-      </c>
-      <c r="O16" s="41">
-        <f t="shared" si="3"/>
-        <v>0.70414012738853515</v>
-      </c>
-      <c r="P16" s="41">
-        <f>100*O16</f>
-        <v>70.414012738853515</v>
-      </c>
-    </row>
-    <row r="20" spans="2:19" ht="28" x14ac:dyDescent="0.15">
-      <c r="H20" s="37" t="s">
-        <v>58</v>
+        <v>94.567404426559349</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="B14" s="31"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="45"/>
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="B15" s="31"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="45"/>
+      <c r="O15" s="42"/>
+      <c r="P15" s="42"/>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="45"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+    </row>
+    <row r="17" spans="2:19">
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+    </row>
+    <row r="18" spans="2:19">
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
+    </row>
+    <row r="19" spans="2:19">
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+    </row>
+    <row r="20" spans="2:19" ht="28">
+      <c r="B20" s="45"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="H20" s="33" t="s">
+        <v>55</v>
       </c>
       <c r="I20">
         <f>I10/L10</f>
-        <v>0.49012738853503185</v>
+        <v>1.0435949027498324</v>
       </c>
       <c r="J20">
         <f>J10/L10</f>
-        <v>2.0847133757961784</v>
+        <v>1.0496311200536554</v>
       </c>
       <c r="K20">
         <f>K10/L10</f>
-        <v>0.42515923566878983</v>
+        <v>0.90677397719651232</v>
       </c>
       <c r="L20">
         <f>AVERAGE(I20:K20)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:19">
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="45"/>
+    </row>
+    <row r="22" spans="2:19">
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="45"/>
+    </row>
+    <row r="23" spans="2:19">
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="45"/>
       <c r="I23">
         <f>I20*100</f>
-        <v>49.012738853503187</v>
+        <v>104.35949027498323</v>
       </c>
       <c r="J23">
         <f>J20*100</f>
-        <v>208.47133757961785</v>
+        <v>104.96311200536555</v>
       </c>
       <c r="K23">
         <f>K20*100</f>
-        <v>42.515923566878982</v>
+        <v>90.677397719651225</v>
       </c>
       <c r="L23">
         <f>AVERAGE(I23:K23)</f>
-        <v>100.00000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="2:19" ht="14" x14ac:dyDescent="0.15">
-      <c r="H26" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="I26" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="K26" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="N26" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="O26" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="P26" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q26" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="R26" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="S26" s="34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="H27" s="34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19">
+      <c r="B24" s="44"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="45"/>
+    </row>
+    <row r="25" spans="2:19">
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+    </row>
+    <row r="26" spans="2:19" ht="14">
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="H26" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="K26" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="P26" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q26" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="R26" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="S26" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19">
+      <c r="H27" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27" s="36">
+        <f>I9/L$10</f>
+        <v>0.78403755868544589</v>
+      </c>
+      <c r="J27" s="36">
+        <f>J9/L$10</f>
+        <v>1.0214621059691482</v>
+      </c>
+      <c r="K27" s="36">
+        <f>K9/L$10</f>
+        <v>0.77397719651240771</v>
+      </c>
+      <c r="N27" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="O27" s="36">
+        <f>I27*100</f>
+        <v>78.403755868544593</v>
+      </c>
+      <c r="P27" s="36">
+        <f>J27*100</f>
+        <v>102.14621059691483</v>
+      </c>
+      <c r="Q27" s="36">
+        <f>+K27*100</f>
+        <v>77.397719651240777</v>
+      </c>
+      <c r="R27" s="36">
+        <f>AVERAGE(O$27:Q$27)</f>
+        <v>85.98256203890007</v>
+      </c>
+      <c r="S27" s="36">
+        <f>STDEV(O$27:R$27)</f>
+        <v>11.436802532406492</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19">
+      <c r="H28" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="I27" s="41">
-        <f>I9/L$10</f>
-        <v>0.36687898089171977</v>
-      </c>
-      <c r="J27" s="41">
-        <f>J9/L$10</f>
-        <v>0.72898089171974523</v>
-      </c>
-      <c r="K27" s="41">
-        <f>K9/L$10</f>
-        <v>0.36210191082802551</v>
-      </c>
-      <c r="N27" s="34" t="s">
+      <c r="I28" s="36">
+        <f t="shared" ref="I28:I34" si="3">I10/L$10</f>
+        <v>1.0435949027498324</v>
+      </c>
+      <c r="J28" s="36">
+        <f t="shared" ref="J28:J34" si="4">J10/L$10</f>
+        <v>1.0496311200536554</v>
+      </c>
+      <c r="K28" s="36">
+        <f t="shared" ref="K28:K34" si="5">K10/L$10</f>
+        <v>0.90677397719651232</v>
+      </c>
+      <c r="N28" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="O27" s="41">
-        <f>I27*100</f>
-        <v>36.687898089171981</v>
-      </c>
-      <c r="P27" s="41">
-        <f>J27*100</f>
-        <v>72.898089171974519</v>
-      </c>
-      <c r="Q27" s="41">
-        <f>+K27*100</f>
-        <v>36.210191082802552</v>
-      </c>
-      <c r="R27" s="41">
-        <f>AVERAGE(O$27:Q$27)</f>
-        <v>48.598726114649686</v>
-      </c>
-      <c r="S27" s="41">
-        <f>STDEV(O$27:R$27)</f>
-        <v>17.183351142695184</v>
-      </c>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="H28" s="34" t="s">
+      <c r="O28" s="36">
+        <f t="shared" ref="O28:O34" si="6">I28*100</f>
+        <v>104.35949027498323</v>
+      </c>
+      <c r="P28" s="36">
+        <f t="shared" ref="P28:P34" si="7">J28*100</f>
+        <v>104.96311200536555</v>
+      </c>
+      <c r="Q28" s="36">
+        <f t="shared" ref="Q28:Q34" si="8">+K28*100</f>
+        <v>90.677397719651225</v>
+      </c>
+      <c r="R28" s="36">
+        <f>AVERAGE(O$28:Q$28)</f>
+        <v>100</v>
+      </c>
+      <c r="S28" s="36">
+        <f>STDEV(O$28:R$28)</f>
+        <v>6.596679708081461</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19">
+      <c r="H29" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="I28" s="41">
-        <f t="shared" ref="I28:I34" si="4">I10/L$10</f>
-        <v>0.49012738853503185</v>
-      </c>
-      <c r="J28" s="41">
-        <f t="shared" ref="J28:J34" si="5">J10/L$10</f>
-        <v>2.0847133757961784</v>
-      </c>
-      <c r="K28" s="41">
-        <f t="shared" ref="K28:K34" si="6">K10/L$10</f>
-        <v>0.42515923566878983</v>
-      </c>
-      <c r="N28" s="34" t="s">
+      <c r="I29" s="36">
+        <f t="shared" si="3"/>
+        <v>0.68745808182427892</v>
+      </c>
+      <c r="J29" s="36">
+        <f t="shared" si="4"/>
+        <v>0.53655264922870549</v>
+      </c>
+      <c r="K29" s="36">
+        <f t="shared" si="5"/>
+        <v>0.50435949027498317</v>
+      </c>
+      <c r="N29" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="O28" s="41">
-        <f t="shared" ref="O28:O34" si="7">I28*100</f>
-        <v>49.012738853503187</v>
-      </c>
-      <c r="P28" s="41">
-        <f t="shared" ref="P28:P34" si="8">J28*100</f>
-        <v>208.47133757961785</v>
-      </c>
-      <c r="Q28" s="41">
-        <f t="shared" ref="Q28:Q34" si="9">+K28*100</f>
-        <v>42.515923566878982</v>
-      </c>
-      <c r="R28" s="41">
-        <f>AVERAGE(O$28:Q$28)</f>
-        <v>100.00000000000001</v>
-      </c>
-      <c r="S28" s="41">
-        <f>STDEV(O$28:R$28)</f>
-        <v>76.746663160690304</v>
-      </c>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="H29" s="34" t="s">
+      <c r="O29" s="36">
+        <f t="shared" si="6"/>
+        <v>68.745808182427893</v>
+      </c>
+      <c r="P29" s="36">
+        <f t="shared" si="7"/>
+        <v>53.65526492287055</v>
+      </c>
+      <c r="Q29" s="36">
+        <f t="shared" si="8"/>
+        <v>50.435949027498317</v>
+      </c>
+      <c r="R29" s="36">
+        <f>AVERAGE(O$29:Q$29)</f>
+        <v>57.612340710932251</v>
+      </c>
+      <c r="S29" s="36">
+        <f>STDEV(O$29:R$29)</f>
+        <v>7.9815024551641942</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19">
+      <c r="H30" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I29" s="41">
+      <c r="I30" s="36">
+        <f t="shared" si="3"/>
+        <v>0.75788061703554654</v>
+      </c>
+      <c r="J30" s="36">
         <f t="shared" si="4"/>
-        <v>0.32101910828025482</v>
-      </c>
-      <c r="J29" s="41">
+        <v>0.94299128101944996</v>
+      </c>
+      <c r="K30" s="36">
         <f t="shared" si="5"/>
-        <v>0.24936305732484079</v>
-      </c>
-      <c r="K29" s="41">
+        <v>0.85244802146210596</v>
+      </c>
+      <c r="N30" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O30" s="36">
         <f t="shared" si="6"/>
-        <v>0.23407643312101911</v>
-      </c>
-      <c r="N29" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="O29" s="41">
+        <v>75.788061703554661</v>
+      </c>
+      <c r="P30" s="36">
         <f t="shared" si="7"/>
-        <v>32.101910828025481</v>
-      </c>
-      <c r="P29" s="41">
+        <v>94.299128101945001</v>
+      </c>
+      <c r="Q30" s="36">
         <f t="shared" si="8"/>
-        <v>24.93630573248408</v>
-      </c>
-      <c r="Q29" s="41">
-        <f t="shared" si="9"/>
-        <v>23.407643312101911</v>
-      </c>
-      <c r="R29" s="41">
-        <f>AVERAGE(O$29:Q$29)</f>
-        <v>26.815286624203821</v>
-      </c>
-      <c r="S29" s="41">
-        <f>STDEV(O$29:R$29)</f>
-        <v>3.7899427263216001</v>
-      </c>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="34" t="s">
+        <v>85.244802146210603</v>
+      </c>
+      <c r="R30" s="36">
+        <f>AVERAGE(O$30:Q$30)</f>
+        <v>85.110663983903422</v>
+      </c>
+      <c r="S30" s="36">
+        <f>STDEV(O30:R30)</f>
+        <v>7.5577064239685994</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19">
+      <c r="H31" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="I30" s="41">
+      <c r="I31" s="36">
+        <f t="shared" si="3"/>
+        <v>0.83433936955063714</v>
+      </c>
+      <c r="J31" s="36">
         <f t="shared" si="4"/>
-        <v>0.35445859872611468</v>
-      </c>
-      <c r="J30" s="41">
+        <v>0.90476190476190466</v>
+      </c>
+      <c r="K31" s="36">
         <f t="shared" si="5"/>
-        <v>0.44235668789808918</v>
-      </c>
-      <c r="K30" s="41">
+        <v>1.0979208584842386</v>
+      </c>
+      <c r="N31" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="O31" s="36">
         <f t="shared" si="6"/>
-        <v>0.39936305732484079</v>
-      </c>
-      <c r="N30" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="O30" s="41">
+        <v>83.433936955063714</v>
+      </c>
+      <c r="P31" s="36">
         <f t="shared" si="7"/>
-        <v>35.445859872611472</v>
-      </c>
-      <c r="P30" s="41">
+        <v>90.476190476190467</v>
+      </c>
+      <c r="Q31" s="36">
         <f t="shared" si="8"/>
-        <v>44.235668789808919</v>
-      </c>
-      <c r="Q30" s="41">
-        <f t="shared" si="9"/>
-        <v>39.93630573248408</v>
-      </c>
-      <c r="R30" s="41">
-        <f>AVERAGE(O$30:Q$30)</f>
-        <v>39.872611464968152</v>
-      </c>
-      <c r="S30" s="41">
-        <f>STDEV(O30:R30)</f>
-        <v>3.5887070949481452</v>
-      </c>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="I31" s="41">
-        <f t="shared" si="4"/>
-        <v>0.39076433121019111</v>
-      </c>
-      <c r="J31" s="41">
-        <f t="shared" si="5"/>
-        <v>0.42420382165605097</v>
-      </c>
-      <c r="K31" s="41">
-        <f t="shared" si="6"/>
-        <v>0.51592356687898089</v>
-      </c>
-      <c r="N31" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="O31" s="41">
-        <f t="shared" si="7"/>
-        <v>39.076433121019107</v>
-      </c>
-      <c r="P31" s="41">
-        <f t="shared" si="8"/>
-        <v>42.420382165605098</v>
-      </c>
-      <c r="Q31" s="41">
-        <f t="shared" si="9"/>
-        <v>51.592356687898089</v>
-      </c>
-      <c r="R31" s="41">
+        <v>109.79208584842385</v>
+      </c>
+      <c r="R31" s="36">
         <f>AVERAGE(O$31:Q31)</f>
-        <v>44.36305732484076</v>
-      </c>
-      <c r="S31" s="41">
+        <v>94.567404426559349</v>
+      </c>
+      <c r="S31" s="36">
         <f>STDEV(O31:R31)</f>
-        <v>5.2910349185342955</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32" s="41">
-        <f t="shared" si="4"/>
-        <v>-2.8662420382165633E-3</v>
-      </c>
-      <c r="J32" s="41">
-        <f t="shared" si="5"/>
-        <v>-4.7770700636942656E-3</v>
-      </c>
-      <c r="K32" s="41">
-        <f t="shared" si="6"/>
-        <v>-2.8662420382165633E-3</v>
-      </c>
-      <c r="N32" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="O32" s="41">
-        <f t="shared" si="7"/>
-        <v>-0.28662420382165632</v>
-      </c>
-      <c r="P32" s="41">
-        <f t="shared" si="8"/>
-        <v>-0.47770700636942653</v>
-      </c>
-      <c r="Q32" s="41">
-        <f t="shared" si="9"/>
-        <v>-0.28662420382165632</v>
-      </c>
-      <c r="R32" s="41">
-        <f>AVERAGE(O32:Q32)</f>
-        <v>-0.35031847133757976</v>
-      </c>
-      <c r="S32" s="41">
-        <f>STDEV(O32:R32)</f>
-        <v>9.0077296966438777E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="I33" s="41">
-        <f t="shared" si="4"/>
-        <v>4.7770700636942656E-3</v>
-      </c>
-      <c r="J33" s="41">
-        <f t="shared" si="5"/>
-        <v>4.7770700636942656E-3</v>
-      </c>
-      <c r="K33" s="41">
-        <f t="shared" si="6"/>
-        <v>5.7324840764331197E-3</v>
-      </c>
-      <c r="N33" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="O33" s="41">
-        <f t="shared" si="7"/>
-        <v>0.47770700636942653</v>
-      </c>
-      <c r="P33" s="41">
-        <f t="shared" si="8"/>
-        <v>0.47770700636942653</v>
-      </c>
-      <c r="Q33" s="41">
-        <f t="shared" si="9"/>
-        <v>0.57324840764331197</v>
-      </c>
-      <c r="R33" s="41">
-        <f>AVERAGE(O33:Q33)</f>
-        <v>0.50955414012738831</v>
-      </c>
-      <c r="S33" s="41">
-        <f>STDEV(O33:R33)</f>
-        <v>4.5038648483219625E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="I34" s="41">
-        <f t="shared" si="4"/>
-        <v>1.3375796178343951</v>
-      </c>
-      <c r="J34" s="41">
-        <f t="shared" si="5"/>
-        <v>0.39554140127388537</v>
-      </c>
-      <c r="K34" s="41">
-        <f t="shared" si="6"/>
-        <v>0.37929936305732487</v>
-      </c>
-      <c r="N34" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="O34" s="41">
-        <f t="shared" si="7"/>
-        <v>133.7579617834395</v>
-      </c>
-      <c r="P34" s="41">
-        <f t="shared" si="8"/>
-        <v>39.554140127388536</v>
-      </c>
-      <c r="Q34" s="41">
-        <f t="shared" si="9"/>
-        <v>37.92993630573249</v>
-      </c>
-      <c r="R34" s="41">
-        <f>AVERAGE(O34:Q34)</f>
-        <v>70.414012738853515</v>
-      </c>
-      <c r="S34" s="41">
-        <f>STDEV(O34:R34)</f>
-        <v>44.795843705533649</v>
-      </c>
-    </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-    </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B36" s="35"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="35"/>
-    </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B37" s="35"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="35"/>
-    </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B38" s="35"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="35"/>
-    </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B39" s="35"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="35"/>
-    </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B40" s="35"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="35"/>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B41" s="35"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="35"/>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B42" s="35"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="35"/>
-    </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B43" s="35"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="35"/>
-    </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B44" s="35"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="35"/>
-    </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B45" s="35"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="35"/>
-    </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B46" s="35"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="35"/>
-    </row>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B47" s="35"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="35"/>
-    </row>
-    <row r="48" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B48" s="35"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="35"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B49" s="35"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="35"/>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B50" s="35"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="35"/>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B51" s="35"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="35"/>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B52" s="35"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="35"/>
-      <c r="I52" s="35"/>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B53" s="35"/>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="35"/>
-      <c r="I53" s="35"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B54" s="35"/>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
+        <v>11.142756300601901</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19">
+      <c r="H32" s="41"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="42"/>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="42"/>
+    </row>
+    <row r="33" spans="3:19">
+      <c r="H33" s="41"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="42"/>
+      <c r="Q33" s="42"/>
+      <c r="R33" s="42"/>
+      <c r="S33" s="42"/>
+    </row>
+    <row r="34" spans="3:19">
+      <c r="H34" s="41"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="42"/>
+      <c r="Q34" s="42"/>
+      <c r="R34" s="42"/>
+      <c r="S34" s="42"/>
+    </row>
+    <row r="36" spans="3:19">
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+    </row>
+    <row r="37" spans="3:19">
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="32"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+    </row>
+    <row r="38" spans="3:19">
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+    </row>
+    <row r="39" spans="3:19">
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+    </row>
+    <row r="40" spans="3:19">
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+    </row>
+    <row r="41" spans="3:19">
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+    </row>
+    <row r="42" spans="3:19">
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+    </row>
+    <row r="43" spans="3:19">
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+    </row>
+    <row r="44" spans="3:19">
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+    </row>
+    <row r="45" spans="3:19">
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+    </row>
+    <row r="46" spans="3:19">
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+    </row>
+    <row r="47" spans="3:19">
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+    </row>
+    <row r="48" spans="3:19">
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+    </row>
+    <row r="49" spans="3:8">
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+    </row>
+    <row r="50" spans="3:8">
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+    </row>
+    <row r="51" spans="3:8">
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3553,115 +3375,222 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{921740F0-408A-5A43-B9FB-E0A88CE3A12D}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="36">
+        <v>100</v>
+      </c>
+      <c r="C2" s="36">
+        <v>6.596679708081461</v>
+      </c>
+      <c r="D2" s="36">
+        <f>AVERAGE(F2:H2)</f>
+        <v>0.13666666666666669</v>
+      </c>
+      <c r="E2" s="36">
+        <v>0.12909944487358077</v>
+      </c>
+      <c r="F2" s="35">
+        <v>0.09</v>
+      </c>
+      <c r="G2" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="36">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="41">
-        <v>48.598726114649686</v>
-      </c>
-      <c r="C2" s="41">
-        <v>17.183351142695184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="41">
-        <v>100</v>
-      </c>
-      <c r="C3" s="41">
-        <v>76.746663160690304</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="41">
-        <v>26.815286624203821</v>
-      </c>
-      <c r="C4" s="41">
-        <v>3.7899427263216001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="41">
-        <v>39.872611464968159</v>
-      </c>
-      <c r="C5" s="41">
-        <v>3.5887070949481452</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="41">
-        <v>44.36305732484076</v>
-      </c>
-      <c r="C6" s="41">
-        <v>5.2910349185342955</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="41">
-        <v>-0.35031847133757971</v>
-      </c>
-      <c r="C7" s="41">
-        <v>9.0077296966438777E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="41">
-        <v>0.50955414012738831</v>
-      </c>
-      <c r="C8" s="41">
-        <v>4.5038648483219625E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="41">
-        <v>70.414012738853515</v>
-      </c>
-      <c r="C9" s="41">
-        <v>44.795843705533649</v>
-      </c>
+      <c r="B3" s="36">
+        <v>85.982562038900056</v>
+      </c>
+      <c r="C3" s="36">
+        <v>11.436802532406492</v>
+      </c>
+      <c r="D3" s="36">
+        <f t="shared" ref="D3:D6" si="0">AVERAGE(F3:H3)</f>
+        <v>0.32333333333333331</v>
+      </c>
+      <c r="E3" s="36">
+        <v>2.1602468994692869E-2</v>
+      </c>
+      <c r="F3" s="36">
+        <v>0.33</v>
+      </c>
+      <c r="G3" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="H3" s="36">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="36">
+        <v>57.612340710932251</v>
+      </c>
+      <c r="C4" s="36">
+        <v>7.9815024551641942</v>
+      </c>
+      <c r="D4" s="36">
+        <f t="shared" si="0"/>
+        <v>51.183333333333337</v>
+      </c>
+      <c r="E4" s="36">
+        <v>15.791749604003879</v>
+      </c>
+      <c r="F4" s="35">
+        <v>46.83</v>
+      </c>
+      <c r="G4" s="36">
+        <v>45.45</v>
+      </c>
+      <c r="H4" s="36">
+        <v>61.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="36">
+        <v>85.110663983903407</v>
+      </c>
+      <c r="C5" s="36">
+        <v>7.5577064239685994</v>
+      </c>
+      <c r="D5" s="36">
+        <f t="shared" si="0"/>
+        <v>43.426666666666669</v>
+      </c>
+      <c r="E5" s="36">
+        <v>5.0228876157047218</v>
+      </c>
+      <c r="F5" s="36">
+        <v>48.52</v>
+      </c>
+      <c r="G5" s="36">
+        <v>45.28</v>
+      </c>
+      <c r="H5" s="36">
+        <v>36.479999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="36">
+        <v>94.567404426559349</v>
+      </c>
+      <c r="C6" s="36">
+        <v>11.142756300601901</v>
+      </c>
+      <c r="D6" s="36">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E6" s="36">
+        <v>0.40088679477156913</v>
+      </c>
+      <c r="F6" s="36">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G6" s="36">
+        <v>0.11</v>
+      </c>
+      <c r="H6" s="36">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="31"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="J7" s="36"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="31"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="31"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="42"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="41"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="42"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>